<commit_message>
实现如下调度的失败重试机制: 1. job_dm_path_parser 1. job_dm_path2object 1. job_dm_obj_metadata 1. job_dm_obj_detail
Signed-off-by: wxy <wangxiya@me.com>
</commit_message>
<xml_diff>
--- a/docs/插件列表.xlsx
+++ b/docs/插件列表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\python_workspace\imetadata\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiya/Documents/Develop/tsdb/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC579D3-9D62-4C32-8571-F049F2D2182C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D5BAE-4DCB-AC42-B8D4-E14839156B06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19740" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="插件列表-识别质检" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'插件列表-识别质检'!$A$2:$AH$118</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -992,23 +992,44 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="宋体"/>
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>王学谦:</t>
+          <t>王学谦</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="宋体"/>
             <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-黄色为做好了没有测试数据，未进行测试</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>黄色为做好了没有测试数据，未进行测试</t>
         </r>
       </text>
     </comment>
@@ -2542,7 +2563,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2735,21 +2756,6 @@
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
       <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3316,32 +3322,32 @@
   </sheetPr>
   <dimension ref="A1:AR119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M97" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="S83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O108" sqref="O108:X108"/>
+      <selection pane="bottomRight" activeCell="V119" sqref="V119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="11.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="11.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.44140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="14" width="20.77734375" customWidth="1"/>
-    <col min="15" max="17" width="21.109375" customWidth="1"/>
-    <col min="18" max="18" width="21.109375" style="12" customWidth="1"/>
-    <col min="19" max="34" width="21.109375" customWidth="1"/>
-    <col min="35" max="35" width="20.77734375" customWidth="1"/>
+    <col min="11" max="14" width="20.83203125" customWidth="1"/>
+    <col min="15" max="17" width="21.1640625" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="12" customWidth="1"/>
+    <col min="19" max="34" width="21.1640625" customWidth="1"/>
+    <col min="35" max="35" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="22" customHeight="1">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -3397,7 +3403,7 @@
       <c r="AQ1" s="50"/>
       <c r="AR1" s="50"/>
     </row>
-    <row r="2" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" ht="22" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
@@ -3531,7 +3537,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="22" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -3615,7 +3621,7 @@
       <c r="AQ3" s="8"/>
       <c r="AR3" s="8"/>
     </row>
-    <row r="4" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="22" customHeight="1">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -3699,7 +3705,7 @@
       <c r="AQ4" s="8"/>
       <c r="AR4" s="8"/>
     </row>
-    <row r="5" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="22" customHeight="1">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -3781,7 +3787,7 @@
       <c r="AQ5" s="8"/>
       <c r="AR5" s="8"/>
     </row>
-    <row r="6" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="22" customHeight="1">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -3863,7 +3869,7 @@
       <c r="AQ6" s="8"/>
       <c r="AR6" s="8"/>
     </row>
-    <row r="7" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="22" customHeight="1">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -3947,7 +3953,7 @@
       <c r="AQ7" s="8"/>
       <c r="AR7" s="8"/>
     </row>
-    <row r="8" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="22" customHeight="1">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -4031,7 +4037,7 @@
       <c r="AQ8" s="8"/>
       <c r="AR8" s="8"/>
     </row>
-    <row r="9" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="22" customHeight="1">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -4113,7 +4119,7 @@
       <c r="AQ9" s="8"/>
       <c r="AR9" s="8"/>
     </row>
-    <row r="10" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="22" customHeight="1">
       <c r="A10" s="14">
         <v>8</v>
       </c>
@@ -4195,7 +4201,7 @@
       <c r="AQ10" s="8"/>
       <c r="AR10" s="8"/>
     </row>
-    <row r="11" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" ht="22" customHeight="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -4277,7 +4283,7 @@
       <c r="AQ11" s="8"/>
       <c r="AR11" s="8"/>
     </row>
-    <row r="12" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" ht="22" customHeight="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -4361,7 +4367,7 @@
       <c r="AQ12" s="8"/>
       <c r="AR12" s="8"/>
     </row>
-    <row r="13" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="22" customHeight="1">
       <c r="A13" s="14">
         <v>11</v>
       </c>
@@ -4445,7 +4451,7 @@
       <c r="AQ13" s="8"/>
       <c r="AR13" s="8"/>
     </row>
-    <row r="14" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="22" customHeight="1">
       <c r="A14" s="14">
         <v>12</v>
       </c>
@@ -4529,7 +4535,7 @@
       <c r="AQ14" s="8"/>
       <c r="AR14" s="8"/>
     </row>
-    <row r="15" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="22" customHeight="1">
       <c r="A15" s="14">
         <v>13</v>
       </c>
@@ -4613,7 +4619,7 @@
       <c r="AQ15" s="8"/>
       <c r="AR15" s="8"/>
     </row>
-    <row r="16" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" ht="22" customHeight="1">
       <c r="A16" s="14">
         <v>14</v>
       </c>
@@ -4697,7 +4703,7 @@
       <c r="AQ16" s="8"/>
       <c r="AR16" s="8"/>
     </row>
-    <row r="17" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" ht="22" customHeight="1">
       <c r="A17" s="14">
         <v>15</v>
       </c>
@@ -4781,7 +4787,7 @@
       <c r="AQ17" s="8"/>
       <c r="AR17" s="8"/>
     </row>
-    <row r="18" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" ht="22" customHeight="1">
       <c r="A18" s="14">
         <v>16</v>
       </c>
@@ -4863,7 +4869,7 @@
       <c r="AQ18" s="8"/>
       <c r="AR18" s="8"/>
     </row>
-    <row r="19" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" ht="22" customHeight="1">
       <c r="A19" s="14">
         <v>17</v>
       </c>
@@ -4945,7 +4951,7 @@
       <c r="AQ19" s="8"/>
       <c r="AR19" s="8"/>
     </row>
-    <row r="20" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" ht="22" customHeight="1">
       <c r="A20" s="14">
         <v>18</v>
       </c>
@@ -5027,7 +5033,7 @@
       <c r="AQ20" s="8"/>
       <c r="AR20" s="8"/>
     </row>
-    <row r="21" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" ht="22" customHeight="1">
       <c r="A21" s="14">
         <v>19</v>
       </c>
@@ -5109,7 +5115,7 @@
       <c r="AQ21" s="8"/>
       <c r="AR21" s="8"/>
     </row>
-    <row r="22" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" ht="22" customHeight="1">
       <c r="A22" s="14">
         <v>20</v>
       </c>
@@ -5191,7 +5197,7 @@
       <c r="AQ22" s="8"/>
       <c r="AR22" s="8"/>
     </row>
-    <row r="23" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" ht="22" customHeight="1">
       <c r="A23" s="14">
         <v>21</v>
       </c>
@@ -5273,7 +5279,7 @@
       <c r="AQ23" s="8"/>
       <c r="AR23" s="8"/>
     </row>
-    <row r="24" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" ht="22" customHeight="1">
       <c r="A24" s="14">
         <v>22</v>
       </c>
@@ -5355,7 +5361,7 @@
       <c r="AQ24" s="8"/>
       <c r="AR24" s="8"/>
     </row>
-    <row r="25" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" ht="22" customHeight="1">
       <c r="A25" s="14">
         <v>23</v>
       </c>
@@ -5437,7 +5443,7 @@
       <c r="AQ25" s="8"/>
       <c r="AR25" s="8"/>
     </row>
-    <row r="26" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" ht="22" customHeight="1">
       <c r="A26" s="14">
         <v>24</v>
       </c>
@@ -5519,7 +5525,7 @@
       <c r="AQ26" s="8"/>
       <c r="AR26" s="8"/>
     </row>
-    <row r="27" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" ht="22" customHeight="1">
       <c r="A27" s="14">
         <v>25</v>
       </c>
@@ -5601,7 +5607,7 @@
       <c r="AQ27" s="8"/>
       <c r="AR27" s="8"/>
     </row>
-    <row r="28" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" ht="22" customHeight="1">
       <c r="A28" s="14">
         <v>26</v>
       </c>
@@ -5683,7 +5689,7 @@
       <c r="AQ28" s="8"/>
       <c r="AR28" s="8"/>
     </row>
-    <row r="29" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" ht="22" customHeight="1">
       <c r="A29" s="14">
         <v>27</v>
       </c>
@@ -5765,7 +5771,7 @@
       <c r="AQ29" s="8"/>
       <c r="AR29" s="8"/>
     </row>
-    <row r="30" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" ht="22" customHeight="1">
       <c r="A30" s="14">
         <v>28</v>
       </c>
@@ -5847,7 +5853,7 @@
       <c r="AQ30" s="8"/>
       <c r="AR30" s="8"/>
     </row>
-    <row r="31" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" ht="22" customHeight="1">
       <c r="A31" s="14">
         <v>29</v>
       </c>
@@ -5929,7 +5935,7 @@
       <c r="AQ31" s="8"/>
       <c r="AR31" s="8"/>
     </row>
-    <row r="32" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" ht="22" customHeight="1">
       <c r="A32" s="14">
         <v>30</v>
       </c>
@@ -6011,7 +6017,7 @@
       <c r="AQ32" s="8"/>
       <c r="AR32" s="8"/>
     </row>
-    <row r="33" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" ht="22" customHeight="1">
       <c r="A33" s="14">
         <v>31</v>
       </c>
@@ -6093,7 +6099,7 @@
       <c r="AQ33" s="8"/>
       <c r="AR33" s="8"/>
     </row>
-    <row r="34" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" ht="22" customHeight="1">
       <c r="A34" s="14">
         <v>32</v>
       </c>
@@ -6175,7 +6181,7 @@
       <c r="AQ34" s="8"/>
       <c r="AR34" s="8"/>
     </row>
-    <row r="35" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" ht="22" customHeight="1">
       <c r="A35" s="14">
         <v>33</v>
       </c>
@@ -6257,7 +6263,7 @@
       <c r="AQ35" s="8"/>
       <c r="AR35" s="8"/>
     </row>
-    <row r="36" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" ht="22" customHeight="1">
       <c r="A36" s="14">
         <v>34</v>
       </c>
@@ -6339,7 +6345,7 @@
       <c r="AQ36" s="8"/>
       <c r="AR36" s="8"/>
     </row>
-    <row r="37" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" ht="22" customHeight="1">
       <c r="A37" s="14">
         <v>35</v>
       </c>
@@ -6421,7 +6427,7 @@
       <c r="AQ37" s="8"/>
       <c r="AR37" s="8"/>
     </row>
-    <row r="38" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" ht="22" customHeight="1">
       <c r="A38" s="14">
         <v>36</v>
       </c>
@@ -6503,7 +6509,7 @@
       <c r="AQ38" s="8"/>
       <c r="AR38" s="8"/>
     </row>
-    <row r="39" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" ht="22" customHeight="1">
       <c r="A39" s="14">
         <v>37</v>
       </c>
@@ -6585,7 +6591,7 @@
       <c r="AQ39" s="8"/>
       <c r="AR39" s="8"/>
     </row>
-    <row r="40" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" ht="22" customHeight="1">
       <c r="A40" s="14">
         <v>38</v>
       </c>
@@ -6667,7 +6673,7 @@
       <c r="AQ40" s="8"/>
       <c r="AR40" s="8"/>
     </row>
-    <row r="41" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" ht="22" customHeight="1">
       <c r="A41" s="14">
         <v>39</v>
       </c>
@@ -6749,7 +6755,7 @@
       <c r="AQ41" s="8"/>
       <c r="AR41" s="8"/>
     </row>
-    <row r="42" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" ht="22" customHeight="1">
       <c r="A42" s="14">
         <v>40</v>
       </c>
@@ -6831,7 +6837,7 @@
       <c r="AQ42" s="8"/>
       <c r="AR42" s="8"/>
     </row>
-    <row r="43" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" ht="22" customHeight="1">
       <c r="A43" s="14">
         <v>41</v>
       </c>
@@ -6913,7 +6919,7 @@
       <c r="AQ43" s="8"/>
       <c r="AR43" s="8"/>
     </row>
-    <row r="44" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" ht="22" customHeight="1">
       <c r="A44" s="14">
         <v>42</v>
       </c>
@@ -6995,7 +7001,7 @@
       <c r="AQ44" s="8"/>
       <c r="AR44" s="8"/>
     </row>
-    <row r="45" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" ht="22" customHeight="1">
       <c r="A45" s="14">
         <v>43</v>
       </c>
@@ -7077,7 +7083,7 @@
       <c r="AQ45" s="8"/>
       <c r="AR45" s="8"/>
     </row>
-    <row r="46" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" ht="22" customHeight="1">
       <c r="A46" s="14">
         <v>44</v>
       </c>
@@ -7159,7 +7165,7 @@
       <c r="AQ46" s="8"/>
       <c r="AR46" s="8"/>
     </row>
-    <row r="47" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" ht="20" customHeight="1">
       <c r="A47" s="14">
         <v>45</v>
       </c>
@@ -7239,7 +7245,7 @@
       <c r="AQ47" s="8"/>
       <c r="AR47" s="8"/>
     </row>
-    <row r="48" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" ht="20" customHeight="1">
       <c r="A48" s="14">
         <v>46</v>
       </c>
@@ -7319,7 +7325,7 @@
       <c r="AQ48" s="8"/>
       <c r="AR48" s="8"/>
     </row>
-    <row r="49" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" ht="20" customHeight="1">
       <c r="A49" s="14">
         <v>47</v>
       </c>
@@ -7399,7 +7405,7 @@
       <c r="AQ49" s="8"/>
       <c r="AR49" s="8"/>
     </row>
-    <row r="50" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:44" ht="20" customHeight="1">
       <c r="A50" s="14">
         <v>48</v>
       </c>
@@ -7479,7 +7485,7 @@
       <c r="AQ50" s="8"/>
       <c r="AR50" s="8"/>
     </row>
-    <row r="51" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" ht="20" customHeight="1">
       <c r="A51" s="14">
         <v>49</v>
       </c>
@@ -7559,7 +7565,7 @@
       <c r="AQ51" s="8"/>
       <c r="AR51" s="8"/>
     </row>
-    <row r="52" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:44" ht="20" customHeight="1">
       <c r="A52" s="14">
         <v>50</v>
       </c>
@@ -7639,7 +7645,7 @@
       <c r="AQ52" s="8"/>
       <c r="AR52" s="8"/>
     </row>
-    <row r="53" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" ht="20" customHeight="1">
       <c r="A53" s="14">
         <v>51</v>
       </c>
@@ -7719,7 +7725,7 @@
       <c r="AQ53" s="8"/>
       <c r="AR53" s="8"/>
     </row>
-    <row r="54" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" ht="20" customHeight="1">
       <c r="A54" s="14">
         <v>52</v>
       </c>
@@ -7799,7 +7805,7 @@
       <c r="AQ54" s="8"/>
       <c r="AR54" s="8"/>
     </row>
-    <row r="55" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" ht="20" customHeight="1">
       <c r="A55" s="14">
         <v>53</v>
       </c>
@@ -7879,7 +7885,7 @@
       <c r="AQ55" s="8"/>
       <c r="AR55" s="8"/>
     </row>
-    <row r="56" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" ht="20" customHeight="1">
       <c r="A56" s="14">
         <v>54</v>
       </c>
@@ -7959,7 +7965,7 @@
       <c r="AQ56" s="8"/>
       <c r="AR56" s="8"/>
     </row>
-    <row r="57" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:44" ht="20" customHeight="1">
       <c r="A57" s="14">
         <v>55</v>
       </c>
@@ -8039,7 +8045,7 @@
       <c r="AQ57" s="8"/>
       <c r="AR57" s="8"/>
     </row>
-    <row r="58" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:44" ht="20" customHeight="1">
       <c r="A58" s="14">
         <v>56</v>
       </c>
@@ -8119,7 +8125,7 @@
       <c r="AQ58" s="8"/>
       <c r="AR58" s="8"/>
     </row>
-    <row r="59" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" ht="20" customHeight="1">
       <c r="A59" s="14">
         <v>57</v>
       </c>
@@ -8199,7 +8205,7 @@
       <c r="AQ59" s="8"/>
       <c r="AR59" s="8"/>
     </row>
-    <row r="60" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" ht="20" customHeight="1">
       <c r="A60" s="14">
         <v>58</v>
       </c>
@@ -8279,7 +8285,7 @@
       <c r="AQ60" s="8"/>
       <c r="AR60" s="8"/>
     </row>
-    <row r="61" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" ht="20" customHeight="1">
       <c r="A61" s="14">
         <v>59</v>
       </c>
@@ -8359,7 +8365,7 @@
       <c r="AQ61" s="8"/>
       <c r="AR61" s="8"/>
     </row>
-    <row r="62" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:44" ht="22" customHeight="1">
       <c r="A62" s="14">
         <v>60</v>
       </c>
@@ -8466,7 +8472,7 @@
       </c>
       <c r="AR62" s="8"/>
     </row>
-    <row r="63" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:44" ht="22" customHeight="1">
       <c r="A63" s="14">
         <v>61</v>
       </c>
@@ -8573,7 +8579,7 @@
       </c>
       <c r="AR63" s="8"/>
     </row>
-    <row r="64" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" ht="22" customHeight="1">
       <c r="A64" s="14">
         <v>62</v>
       </c>
@@ -8680,7 +8686,7 @@
       </c>
       <c r="AR64" s="8"/>
     </row>
-    <row r="65" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:44" ht="22" customHeight="1">
       <c r="A65" s="14">
         <v>63</v>
       </c>
@@ -8787,7 +8793,7 @@
       </c>
       <c r="AR65" s="8"/>
     </row>
-    <row r="66" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:44" ht="22" customHeight="1">
       <c r="A66" s="14">
         <v>64</v>
       </c>
@@ -8894,7 +8900,7 @@
       </c>
       <c r="AR66" s="8"/>
     </row>
-    <row r="67" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" ht="22" customHeight="1">
       <c r="A67" s="14">
         <v>65</v>
       </c>
@@ -9001,7 +9007,7 @@
       </c>
       <c r="AR67" s="8"/>
     </row>
-    <row r="68" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:44" ht="22" customHeight="1">
       <c r="A68" s="14">
         <v>66</v>
       </c>
@@ -9108,7 +9114,7 @@
       </c>
       <c r="AR68" s="8"/>
     </row>
-    <row r="69" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:44" ht="22" customHeight="1">
       <c r="A69" s="14">
         <v>67</v>
       </c>
@@ -9215,7 +9221,7 @@
       </c>
       <c r="AR69" s="8"/>
     </row>
-    <row r="70" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:44" ht="22" customHeight="1">
       <c r="A70" s="14">
         <v>68</v>
       </c>
@@ -9322,7 +9328,7 @@
       </c>
       <c r="AR70" s="8"/>
     </row>
-    <row r="71" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:44" ht="22" customHeight="1">
       <c r="A71" s="14">
         <v>69</v>
       </c>
@@ -9429,7 +9435,7 @@
       </c>
       <c r="AR71" s="8"/>
     </row>
-    <row r="72" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:44" ht="22" customHeight="1">
       <c r="A72" s="14">
         <v>70</v>
       </c>
@@ -9536,7 +9542,7 @@
       </c>
       <c r="AR72" s="8"/>
     </row>
-    <row r="73" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:44" ht="22" customHeight="1">
       <c r="A73" s="14">
         <v>71</v>
       </c>
@@ -9643,7 +9649,7 @@
       </c>
       <c r="AR73" s="8"/>
     </row>
-    <row r="74" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:44" ht="22" customHeight="1">
       <c r="A74" s="14">
         <v>72</v>
       </c>
@@ -9750,7 +9756,7 @@
       </c>
       <c r="AR74" s="8"/>
     </row>
-    <row r="75" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:44" ht="22" customHeight="1">
       <c r="A75" s="14">
         <v>73</v>
       </c>
@@ -9857,7 +9863,7 @@
       </c>
       <c r="AR75" s="8"/>
     </row>
-    <row r="76" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:44" ht="22" customHeight="1">
       <c r="A76" s="14">
         <v>74</v>
       </c>
@@ -9964,7 +9970,7 @@
       </c>
       <c r="AR76" s="8"/>
     </row>
-    <row r="77" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:44" ht="22" customHeight="1">
       <c r="A77" s="14">
         <v>75</v>
       </c>
@@ -10071,7 +10077,7 @@
       </c>
       <c r="AR77" s="8"/>
     </row>
-    <row r="78" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:44" ht="22" customHeight="1">
       <c r="A78" s="14">
         <v>76</v>
       </c>
@@ -10178,7 +10184,7 @@
       </c>
       <c r="AR78" s="8"/>
     </row>
-    <row r="79" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:44" ht="22" customHeight="1">
       <c r="A79" s="14">
         <v>77</v>
       </c>
@@ -10285,7 +10291,7 @@
       </c>
       <c r="AR79" s="8"/>
     </row>
-    <row r="80" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:44" ht="22" customHeight="1">
       <c r="A80" s="14">
         <v>78</v>
       </c>
@@ -10392,7 +10398,7 @@
       </c>
       <c r="AR80" s="8"/>
     </row>
-    <row r="81" spans="1:44" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:44" ht="22" customHeight="1">
       <c r="A81" s="14">
         <v>79</v>
       </c>
@@ -10499,7 +10505,7 @@
       </c>
       <c r="AR81" s="8"/>
     </row>
-    <row r="82" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:44" ht="20" customHeight="1">
       <c r="A82" s="14">
         <v>80</v>
       </c>
@@ -10606,7 +10612,7 @@
       </c>
       <c r="AR82" s="8"/>
     </row>
-    <row r="83" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:44" ht="20" customHeight="1">
       <c r="A83" s="14">
         <v>81</v>
       </c>
@@ -10713,7 +10719,7 @@
       </c>
       <c r="AR83" s="8"/>
     </row>
-    <row r="84" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:44" ht="20" customHeight="1">
       <c r="A84" s="14">
         <v>82</v>
       </c>
@@ -10820,7 +10826,7 @@
       </c>
       <c r="AR84" s="8"/>
     </row>
-    <row r="85" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:44" ht="20" customHeight="1">
       <c r="A85" s="14">
         <v>83</v>
       </c>
@@ -10927,7 +10933,7 @@
       </c>
       <c r="AR85" s="8"/>
     </row>
-    <row r="86" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:44" ht="20" customHeight="1">
       <c r="A86" s="14">
         <v>84</v>
       </c>
@@ -11034,7 +11040,7 @@
       </c>
       <c r="AR86" s="8"/>
     </row>
-    <row r="87" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:44" ht="20" customHeight="1">
       <c r="A87" s="14">
         <v>87</v>
       </c>
@@ -11141,7 +11147,7 @@
       </c>
       <c r="AR87" s="32"/>
     </row>
-    <row r="88" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:44" ht="20" customHeight="1">
       <c r="A88" s="14">
         <v>91</v>
       </c>
@@ -11248,7 +11254,7 @@
       </c>
       <c r="AR88" s="8"/>
     </row>
-    <row r="89" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:44" ht="20" customHeight="1">
       <c r="A89" s="14">
         <v>92</v>
       </c>
@@ -11355,7 +11361,7 @@
       </c>
       <c r="AR89" s="8"/>
     </row>
-    <row r="90" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:44" ht="20" customHeight="1">
       <c r="A90" s="14">
         <v>94</v>
       </c>
@@ -11454,7 +11460,7 @@
       </c>
       <c r="AR90" s="8"/>
     </row>
-    <row r="91" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:44" ht="20" customHeight="1">
       <c r="A91" s="14">
         <v>95</v>
       </c>
@@ -11561,7 +11567,7 @@
       </c>
       <c r="AR91" s="8"/>
     </row>
-    <row r="92" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:44" ht="20" customHeight="1">
       <c r="A92" s="14">
         <v>97</v>
       </c>
@@ -11668,7 +11674,7 @@
       </c>
       <c r="AR92" s="8"/>
     </row>
-    <row r="93" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:44" ht="20" customHeight="1">
       <c r="A93" s="14">
         <v>98</v>
       </c>
@@ -11775,7 +11781,7 @@
       </c>
       <c r="AR93" s="8"/>
     </row>
-    <row r="94" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:44" ht="20" customHeight="1">
       <c r="A94" s="14">
         <v>99</v>
       </c>
@@ -11870,7 +11876,7 @@
       </c>
       <c r="AR94" s="8"/>
     </row>
-    <row r="95" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:44" ht="20" customHeight="1">
       <c r="A95" s="14">
         <v>100</v>
       </c>
@@ -11977,7 +11983,7 @@
       </c>
       <c r="AR95" s="8"/>
     </row>
-    <row r="96" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:44" ht="20" customHeight="1">
       <c r="A96" s="14">
         <v>101</v>
       </c>
@@ -12084,7 +12090,7 @@
       </c>
       <c r="AR96" s="8"/>
     </row>
-    <row r="97" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:44" ht="20" customHeight="1">
       <c r="A97" s="14">
         <v>103</v>
       </c>
@@ -12191,7 +12197,7 @@
       </c>
       <c r="AR97" s="8"/>
     </row>
-    <row r="98" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:44" ht="20" customHeight="1">
       <c r="A98" s="14">
         <v>107</v>
       </c>
@@ -12298,7 +12304,7 @@
       </c>
       <c r="AR98" s="8"/>
     </row>
-    <row r="99" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:44" ht="20" customHeight="1">
       <c r="A99" s="14">
         <v>108</v>
       </c>
@@ -12393,7 +12399,7 @@
       </c>
       <c r="AR99" s="8"/>
     </row>
-    <row r="100" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:44" ht="20" customHeight="1">
       <c r="A100" s="14">
         <v>109</v>
       </c>
@@ -12488,7 +12494,7 @@
       </c>
       <c r="AR100" s="8"/>
     </row>
-    <row r="101" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:44" ht="20" customHeight="1">
       <c r="A101" s="14">
         <v>110</v>
       </c>
@@ -12595,7 +12601,7 @@
       </c>
       <c r="AR101" s="8"/>
     </row>
-    <row r="102" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:44" ht="20" customHeight="1">
       <c r="A102" s="14">
         <v>112</v>
       </c>
@@ -12702,7 +12708,7 @@
       </c>
       <c r="AR102" s="8"/>
     </row>
-    <row r="103" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:44" ht="20" customHeight="1">
       <c r="A103" s="14">
         <v>113</v>
       </c>
@@ -12809,7 +12815,7 @@
       </c>
       <c r="AR103" s="8"/>
     </row>
-    <row r="104" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:44" ht="20" customHeight="1">
       <c r="A104" s="14">
         <v>114</v>
       </c>
@@ -12916,7 +12922,7 @@
       </c>
       <c r="AR104" s="8"/>
     </row>
-    <row r="105" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:44" ht="20" customHeight="1">
       <c r="A105" s="14">
         <v>115</v>
       </c>
@@ -13023,7 +13029,7 @@
       </c>
       <c r="AR105" s="8"/>
     </row>
-    <row r="106" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:44" ht="20" customHeight="1">
       <c r="A106" s="14">
         <v>116</v>
       </c>
@@ -13130,7 +13136,7 @@
       </c>
       <c r="AR106" s="8"/>
     </row>
-    <row r="107" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:44" ht="20" customHeight="1">
       <c r="A107" s="14">
         <v>117</v>
       </c>
@@ -13237,7 +13243,7 @@
       </c>
       <c r="AR107" s="8"/>
     </row>
-    <row r="108" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:44" ht="20" customHeight="1">
       <c r="A108" s="14">
         <v>118</v>
       </c>
@@ -13338,7 +13344,7 @@
       </c>
       <c r="AR108" s="8"/>
     </row>
-    <row r="109" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:44" ht="20" customHeight="1">
       <c r="A109" s="14">
         <v>90</v>
       </c>
@@ -13447,7 +13453,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:44" ht="20" customHeight="1">
       <c r="A110" s="14">
         <v>86</v>
       </c>
@@ -13556,7 +13562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="111" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:44" ht="20" customHeight="1">
       <c r="A111" s="14">
         <v>120</v>
       </c>
@@ -13657,7 +13663,7 @@
       </c>
       <c r="AR111" s="8"/>
     </row>
-    <row r="112" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:44" ht="20" customHeight="1">
       <c r="A112" s="14">
         <v>121</v>
       </c>
@@ -13758,7 +13764,7 @@
       </c>
       <c r="AR112" s="8"/>
     </row>
-    <row r="113" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:44" ht="20" customHeight="1">
       <c r="A113" s="14">
         <v>122</v>
       </c>
@@ -13853,7 +13859,7 @@
       </c>
       <c r="AR113" s="8"/>
     </row>
-    <row r="114" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:44" ht="20" customHeight="1">
       <c r="A114" s="14">
         <v>123</v>
       </c>
@@ -13948,7 +13954,7 @@
       </c>
       <c r="AR114" s="8"/>
     </row>
-    <row r="115" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:44" ht="20" customHeight="1">
       <c r="A115" s="14">
         <v>124</v>
       </c>
@@ -14041,7 +14047,7 @@
       </c>
       <c r="AR115" s="8"/>
     </row>
-    <row r="116" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:44" ht="20" customHeight="1">
       <c r="A116" s="14">
         <v>125</v>
       </c>
@@ -14134,7 +14140,7 @@
       </c>
       <c r="AR116" s="8"/>
     </row>
-    <row r="117" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:44" ht="20" customHeight="1">
       <c r="A117" s="14">
         <v>96</v>
       </c>
@@ -14229,7 +14235,7 @@
       </c>
       <c r="AR117" s="8"/>
     </row>
-    <row r="118" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:44" ht="20" customHeight="1">
       <c r="A118" s="14">
         <v>126</v>
       </c>
@@ -14305,7 +14311,7 @@
       <c r="AQ118" s="8"/>
       <c r="AR118" s="8"/>
     </row>
-    <row r="119" spans="1:44" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:44" ht="20" customHeight="1">
       <c r="F119" s="16" t="s">
         <v>411</v>
       </c>
@@ -14376,11 +14382,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:AH118" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:AH118">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH118">
       <sortCondition ref="C2:C26"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A3:AH17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH17">
     <sortCondition ref="E4:E17"/>
     <sortCondition ref="D4:D17"/>
     <sortCondition ref="G4:G17"/>
@@ -14407,19 +14413,19 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="31" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="26.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -14445,7 +14451,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -14471,7 +14477,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20" customHeight="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -14497,7 +14503,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20" customHeight="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -14523,7 +14529,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20" customHeight="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -14549,7 +14555,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="20" customHeight="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -14575,7 +14581,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="20" customHeight="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -14601,7 +14607,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="20" customHeight="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -14627,7 +14633,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="20" customHeight="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -14653,7 +14659,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="32">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -14679,7 +14685,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18" customHeight="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -14705,7 +14711,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="20" customHeight="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -14731,7 +14737,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="48">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -14757,7 +14763,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="20" customHeight="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -14783,7 +14789,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="20" customHeight="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -14809,7 +14815,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="20" customHeight="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -14835,7 +14841,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="48">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -14861,7 +14867,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="20" customHeight="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -14887,7 +14893,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="20" customHeight="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -14913,7 +14919,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="32">
       <c r="A20" s="5">
         <v>19</v>
       </c>

</xml_diff>